<commit_message>
Añado base de datos y mejoro la legibilidad del codigo
</commit_message>
<xml_diff>
--- a/resultados/excels/amazon/busquedas_amazon.xlsx
+++ b/resultados/excels/amazon/busquedas_amazon.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="217">
   <si>
     <t>Fecha</t>
   </si>
@@ -31,9 +31,15 @@
     <t>URL Producto</t>
   </si>
   <si>
+    <t>Pagina Web</t>
+  </si>
+  <si>
     <t>2025-06-10</t>
   </si>
   <si>
+    <t>2025-06-13</t>
+  </si>
+  <si>
     <t>Taza de cerámica de 325 ml en caja de regalo de Pokemon</t>
   </si>
   <si>
@@ -157,6 +163,27 @@
     <t>Bandai DigimonX (Morado y Rojo) - Mascota Monstruo Virtual por Tamagotchi</t>
   </si>
   <si>
+    <t>Pokémon Lote de Sobres de Mejora de Escarlata y Púrpura-Juntos de Aventuras de JCC Pokémon (6 Sobres de Mejora)</t>
+  </si>
+  <si>
+    <t>Pokémon: Caja de Entrenador Élite de Escarlata y Púrpura-Rivales Predestinados de JCC Pokémon (1 Carta de promoción con ilustración expandida, 9 Sobres de Mejora y Accesorios prémium)</t>
+  </si>
+  <si>
+    <t>Ravensburger - Puzzle 500 Piezas, Pokemon Challenge, Puzzle Adultos 500 Piezas, Rompecabezas, Regalo Pokemon, 49x36cm</t>
+  </si>
+  <si>
+    <t>Pokémon Escarlata/Púrpura El tesoro oculto del Área Cero | Nintendo Switch - Código de descarga</t>
+  </si>
+  <si>
+    <t>Pokémon Lote de Paquetes de Mejora de JCC Pokémon (4 Paquetes de Mejora, 40 Cartas en Total) (Puede Contener Paquetes de Mejora duplicados)</t>
+  </si>
+  <si>
+    <t>Leyendas Pokémon: Z‑A</t>
+  </si>
+  <si>
+    <t>Ravensburger - Puzzle 3d Niños Pokemon Pokeball | Puzzles 3d Para Niños De 6 Años O Más | Maquetas Para Montar De 55 Piezas | Regalo Niño 6 Años O Más</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
@@ -256,6 +283,9 @@
     <t>17</t>
   </si>
   <si>
+    <t>31</t>
+  </si>
+  <si>
     <t>https://m.media-amazon.com/images/I/61K7pJW7-TL._AC_SX679_.jpg</t>
   </si>
   <si>
@@ -397,6 +427,30 @@
     <t>https://m.media-amazon.com/images/I/71-UO4d6WPS.__AC_SY300_SX300_QL70_ML2_.jpg</t>
   </si>
   <si>
+    <t>https://m.media-amazon.com/images/I/81Z-5Zbet-L._AC_SY550_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/81jW+mFahBL._AC_SX425_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/71cSHoKv0EL._AC_SY550_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/81RstjzDTyL._AC_SY741_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/81kM4x8kobL._AC_SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/811A3T+RmJL._AC_SX425_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/619i1Co31wL._AC_SY741_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/61aH2OG043L._AC_SX425_.jpg</t>
+  </si>
+  <si>
     <t>https://www.amazon.es/Taza-Cer%C3%A1mica-325-ml-Pokemon/dp/B0B4636ZN4/ref=sr_1_15</t>
   </si>
   <si>
@@ -563,6 +617,54 @@
   </si>
   <si>
     <t>https://www.amazon.es/Bandai-DigimonX-p%C3%BArpura-Rojo-Tamagotchi/dp/B099CCLZCT/ref=sr_1_31</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Bizak-Charizard-Electr%C3%B3nico-reacciones-Movimiento/dp/B0C3MHJJ6Y/ref=sr_1_39</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Ravensburger-Labyrint-Connect-CartasJuego-Jugadores/dp/B0CSZ172NC/ref=sr_1_36</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Pok%C3%A9mon-JCC-P%C3%BArpura-Llamas-hologr%C3%A1fica-ilustraci%C3%B3n/dp/B0C64HDD6D/ref=sr_1_47</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Pok%C3%A9mon-Lote-Escarlata-P%C3%BArpura-Juntos-Aventuras/dp/B0DZP46367/ref=sr_1_43</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Pok%C3%A9mon-Entrenador-P%C3%BArpura-Rivales-Predestinados-ilustraci%C3%B3n/dp/B0F8BQ3PCL/ref=sr_1_29</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Ravensburger-12000511-primeros-Pok%C3%A9mon-adultos/dp/B0CQ8G4P8P/ref=sr_1_46</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Pok%C3%A9mon-Escarlata-P%C3%BArpura-tesoro-Nintendo/dp/B0BXQK65FX/ref=sr_1_38</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Pok%C3%A9mon-Lote-Paquetes-Contener-duplicados/dp/B0DSG8KDV9/ref=sr_1_45</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Juego-Mesa-Monopoly-Edici%C3%B3n-Pok%C3%A9mon/dp/B0DLJFDZF5/ref=sr_1_37</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Nintendo-Leyendas-Pok%C3%A9mon-Z%E2%80%91A/dp/B0D42BGBV3/ref=sr_1_32</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Ravensburger-Pok%C3%A9mon-Pokeball-Maqueta-Rompecabezas/dp/B08L3XBZ48/ref=sr_1_40</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Pok%C3%A9mon-JCC-P%C3%BArpura-Llamas-hologr%C3%A1fica-ilustraci%C3%B3n/dp/B0C64HDD6D/ref=sr_1_46</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Ravensburger-12000511-primeros-Pok%C3%A9mon-adultos/dp/B0CQ8G4P8P/ref=sr_1_47</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Pok%C3%A9mon-Lote-Paquetes-Contener-duplicados/dp/B0DSG8KDV9/ref=sr_1_44</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/Enciclopedia-Pok%C3%A9mon-Colecci%C3%B3n-Company/dp/8419169269/ref=sr_1_48</t>
+  </si>
+  <si>
+    <t>Amazon</t>
   </si>
 </sst>
 </file>
@@ -933,13 +1035,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -955,1025 +1057,1468 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C42" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s">
+        <v>44</v>
+      </c>
+      <c r="C54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" t="s">
         <v>32</v>
       </c>
-      <c r="C48" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" t="s">
-        <v>76</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="C55" t="s">
+        <v>75</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" t="s">
+        <v>79</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C60" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" t="s">
-        <v>44</v>
-      </c>
-      <c r="C50" t="s">
-        <v>77</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" t="s">
-        <v>37</v>
-      </c>
-      <c r="C51" t="s">
-        <v>71</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" t="s">
-        <v>34</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="E61" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" t="s">
+        <v>67</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F62" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F63" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" t="s">
+        <v>89</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F64" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>49</v>
+      </c>
+      <c r="C65" t="s">
+        <v>79</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F65" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66" t="s">
+        <v>66</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F66" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" t="s">
+        <v>51</v>
+      </c>
+      <c r="C67" t="s">
+        <v>59</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F67" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" t="s">
+        <v>52</v>
+      </c>
+      <c r="C68" t="s">
+        <v>57</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F68" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" t="s">
+        <v>53</v>
+      </c>
+      <c r="C69" t="s">
+        <v>84</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F69" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" t="s">
+        <v>70</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F70" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" t="s">
+        <v>54</v>
+      </c>
+      <c r="C71" t="s">
         <v>68</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53" t="s">
-        <v>45</v>
-      </c>
-      <c r="C53" t="s">
-        <v>78</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" t="s">
-        <v>42</v>
-      </c>
-      <c r="C54" t="s">
-        <v>75</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" t="s">
-        <v>5</v>
-      </c>
-      <c r="B55" t="s">
-        <v>30</v>
-      </c>
-      <c r="C55" t="s">
-        <v>66</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56" t="s">
-        <v>37</v>
-      </c>
-      <c r="C56" t="s">
-        <v>71</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57" t="s">
-        <v>36</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="D71" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F71" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C72" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F72" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" t="s">
+        <v>67</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F73" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" t="s">
+        <v>63</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F74" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" t="s">
+        <v>7</v>
+      </c>
+      <c r="B75" t="s">
+        <v>49</v>
+      </c>
+      <c r="C75" t="s">
+        <v>79</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F75" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" t="s">
+        <v>89</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F76" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77" t="s">
+        <v>51</v>
+      </c>
+      <c r="C77" t="s">
+        <v>59</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F77" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" t="s">
+        <v>7</v>
+      </c>
+      <c r="B78" t="s">
+        <v>52</v>
+      </c>
+      <c r="C78" t="s">
+        <v>57</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F78" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" t="s">
+        <v>53</v>
+      </c>
+      <c r="C79" t="s">
+        <v>84</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F79" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" t="s">
+        <v>7</v>
+      </c>
+      <c r="B80" t="s">
+        <v>26</v>
+      </c>
+      <c r="C80" t="s">
         <v>70</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" t="s">
-        <v>31</v>
-      </c>
-      <c r="C58" t="s">
-        <v>61</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" t="s">
-        <v>62</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" t="s">
-        <v>5</v>
-      </c>
-      <c r="B60" t="s">
-        <v>46</v>
-      </c>
-      <c r="C60" t="s">
-        <v>79</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61" t="s">
-        <v>35</v>
-      </c>
-      <c r="C61" t="s">
-        <v>69</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>162</v>
+      <c r="D80" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F80" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" t="s">
+        <v>7</v>
+      </c>
+      <c r="B81" t="s">
+        <v>54</v>
+      </c>
+      <c r="C81" t="s">
+        <v>68</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F81" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" t="s">
+        <v>7</v>
+      </c>
+      <c r="B82" t="s">
+        <v>55</v>
+      </c>
+      <c r="C82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F82" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" t="s">
+        <v>7</v>
+      </c>
+      <c r="B83" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83" t="s">
+        <v>60</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F83" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2098,6 +2643,50 @@
     <hyperlink ref="E60" r:id="rId118"/>
     <hyperlink ref="D61" r:id="rId119"/>
     <hyperlink ref="E61" r:id="rId120"/>
+    <hyperlink ref="D62" r:id="rId121"/>
+    <hyperlink ref="E62" r:id="rId122"/>
+    <hyperlink ref="D63" r:id="rId123"/>
+    <hyperlink ref="E63" r:id="rId124"/>
+    <hyperlink ref="D64" r:id="rId125"/>
+    <hyperlink ref="E64" r:id="rId126"/>
+    <hyperlink ref="D65" r:id="rId127"/>
+    <hyperlink ref="E65" r:id="rId128"/>
+    <hyperlink ref="D66" r:id="rId129"/>
+    <hyperlink ref="E66" r:id="rId130"/>
+    <hyperlink ref="D67" r:id="rId131"/>
+    <hyperlink ref="E67" r:id="rId132"/>
+    <hyperlink ref="D68" r:id="rId133"/>
+    <hyperlink ref="E68" r:id="rId134"/>
+    <hyperlink ref="D69" r:id="rId135"/>
+    <hyperlink ref="E69" r:id="rId136"/>
+    <hyperlink ref="D70" r:id="rId137"/>
+    <hyperlink ref="E70" r:id="rId138"/>
+    <hyperlink ref="D71" r:id="rId139"/>
+    <hyperlink ref="E71" r:id="rId140"/>
+    <hyperlink ref="D72" r:id="rId141"/>
+    <hyperlink ref="E72" r:id="rId142"/>
+    <hyperlink ref="D73" r:id="rId143"/>
+    <hyperlink ref="E73" r:id="rId144"/>
+    <hyperlink ref="D74" r:id="rId145"/>
+    <hyperlink ref="E74" r:id="rId146"/>
+    <hyperlink ref="D75" r:id="rId147"/>
+    <hyperlink ref="E75" r:id="rId148"/>
+    <hyperlink ref="D76" r:id="rId149"/>
+    <hyperlink ref="E76" r:id="rId150"/>
+    <hyperlink ref="D77" r:id="rId151"/>
+    <hyperlink ref="E77" r:id="rId152"/>
+    <hyperlink ref="D78" r:id="rId153"/>
+    <hyperlink ref="E78" r:id="rId154"/>
+    <hyperlink ref="D79" r:id="rId155"/>
+    <hyperlink ref="E79" r:id="rId156"/>
+    <hyperlink ref="D80" r:id="rId157"/>
+    <hyperlink ref="E80" r:id="rId158"/>
+    <hyperlink ref="D81" r:id="rId159"/>
+    <hyperlink ref="E81" r:id="rId160"/>
+    <hyperlink ref="D82" r:id="rId161"/>
+    <hyperlink ref="E82" r:id="rId162"/>
+    <hyperlink ref="D83" r:id="rId163"/>
+    <hyperlink ref="E83" r:id="rId164"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>